<commit_message>
Changes for ledgers implementation
Changes for ledgers implementation
</commit_message>
<xml_diff>
--- a/01_Requirements/LedgerTypes/011_Raw Material ledgers.xlsx
+++ b/01_Requirements/LedgerTypes/011_Raw Material ledgers.xlsx
@@ -372,18 +372,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -393,77 +387,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,7 +748,7 @@
   <dimension ref="D2:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -765,287 +765,287 @@
     </row>
     <row r="3" spans="4:12" ht="15.75" thickBot="1"/>
     <row r="4" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="9" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="10"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D6" s="5"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="10"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D8" s="5"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D10" s="5"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="11" spans="4:12" ht="24.95" customHeight="1">
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="15" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="10"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="4:12" ht="24.95" customHeight="1">
-      <c r="D12" s="5"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
+      <c r="D12" s="2"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="25"/>
     </row>
     <row r="13" spans="4:12" ht="24.95" customHeight="1">
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="32"/>
+      <c r="G13" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19" t="s">
+      <c r="H13" s="32"/>
+      <c r="I13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="10"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="4:12" ht="24.95" customHeight="1">
-      <c r="D14" s="5"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="10"/>
+      <c r="D14" s="2"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="25"/>
     </row>
     <row r="15" spans="4:12" ht="24.95" customHeight="1">
-      <c r="D15" s="5"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="10"/>
+      <c r="D15" s="2"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="4:12" ht="24.95" customHeight="1">
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="20" t="s">
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="10"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="25"/>
     </row>
     <row r="17" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D17" s="5"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="10"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="10"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D19" s="5"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="10"/>
+      <c r="D19" s="2"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="25"/>
     </row>
     <row r="20" spans="4:12" ht="15.75" thickBot="1">
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="30"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="22" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="4:12" ht="20.100000000000001" customHeight="1">
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="20.100000000000001" customHeight="1">
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="20.100000000000001" customHeight="1">
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="20.100000000000001" customHeight="1">
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="20.100000000000001" customHeight="1">
-      <c r="D36" s="32" t="s">
+      <c r="D36" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="20.100000000000001" customHeight="1">
-      <c r="D37" s="32" t="s">
+      <c r="D37" s="10" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>